<commit_message>
First results, simple approach - corrected staged area
</commit_message>
<xml_diff>
--- a/Locations.xlsx
+++ b/Locations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e46eb1fa8f051fd0/Dokumenty/1_STUDIA/1_UEK/semestr3/Metody_metaheurystyczne/projekt/CVRP_python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="163" documentId="11_F25DC773A252ABDACC104851391E68845BDE58F6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DC2A0E82-FEE2-44D1-A638-6AAAEA4A553D}"/>
+  <xr:revisionPtr revIDLastSave="169" documentId="11_F25DC773A252ABDACC104851391E68845BDE58F6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7BDC91D2-381C-4020-80B0-8FE81F711A5F}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="6450" yWindow="2040" windowWidth="17685" windowHeight="14295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25035" yWindow="4995" windowWidth="17685" windowHeight="12660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>City</t>
   </si>
@@ -127,6 +127,9 @@
   </si>
   <si>
     <t>Zamość</t>
+  </si>
+  <si>
+    <t>Kraków</t>
   </si>
 </sst>
 </file>
@@ -448,10 +451,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -478,421 +481,435 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>34</v>
       </c>
       <c r="B2">
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="C2">
-        <v>53.141523238267197</v>
+        <v>50.062537797834501</v>
       </c>
       <c r="D2">
-        <v>23.1440492704264</v>
+        <v>19.937306291842098</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3">
-        <v>50</v>
+        <v>500</v>
       </c>
       <c r="C3">
-        <v>49.816166686715498</v>
+        <v>53.141523238267197</v>
       </c>
       <c r="D3">
-        <v>19.043440866477699</v>
+        <v>23.1440492704264</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4">
-        <v>400</v>
+        <v>50</v>
       </c>
       <c r="C4">
-        <v>50.138898893478</v>
+        <v>49.816166686715498</v>
       </c>
       <c r="D4">
-        <v>19.400068642432299</v>
+        <v>19.043440866477699</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="C5">
-        <v>54.371007349397701</v>
+        <v>50.138898893478</v>
       </c>
       <c r="D5">
-        <v>18.6035054972849</v>
+        <v>19.400068642432299</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="C6">
-        <v>54.5107669366868</v>
+        <v>54.371007349397701</v>
       </c>
       <c r="D6">
-        <v>18.5245412653586</v>
+        <v>18.6035054972849</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="C7">
-        <v>50.295077875394902</v>
+        <v>54.5107669366868</v>
       </c>
       <c r="D7">
-        <v>18.673647759229901</v>
+        <v>18.5245412653586</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8">
-        <v>200</v>
+        <v>40</v>
       </c>
       <c r="C8">
-        <v>49.838331872741698</v>
+        <v>50.295077875394902</v>
       </c>
       <c r="D8">
-        <v>20.961498232116998</v>
+        <v>18.673647759229901</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B9">
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="C9">
-        <v>50.260215955446398</v>
+        <v>49.838331872741698</v>
       </c>
       <c r="D9">
-        <v>19.018350500255998</v>
+        <v>20.961498232116998</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B10">
-        <v>30</v>
+        <v>300</v>
       </c>
       <c r="C10">
-        <v>50.866603930284597</v>
+        <v>50.260215955446398</v>
       </c>
       <c r="D10">
-        <v>20.627657351131202</v>
+        <v>19.018350500255998</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B11">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="C11">
-        <v>49.689871625475099</v>
+        <v>50.866603930284597</v>
       </c>
       <c r="D11">
-        <v>21.7668695000851</v>
+        <v>20.627657351131202</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B12">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="C12">
-        <v>49.415894571510897</v>
+        <v>49.689871625475099</v>
       </c>
       <c r="D12">
-        <v>20.951569207975901</v>
+        <v>21.7668695000851</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B13">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="C13">
-        <v>51.246250096384401</v>
+        <v>49.415894571510897</v>
       </c>
       <c r="D13">
-        <v>22.570635490611799</v>
+        <v>20.951569207975901</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B14">
-        <v>160</v>
+        <v>60</v>
       </c>
       <c r="C14">
-        <v>51.759498863765302</v>
+        <v>51.246250096384401</v>
       </c>
       <c r="D14">
-        <v>19.456902127582101</v>
+        <v>22.570635490611799</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B15">
-        <v>100</v>
+        <v>160</v>
       </c>
       <c r="C15">
-        <v>54.035961601523603</v>
+        <v>51.759498863765302</v>
       </c>
       <c r="D15">
-        <v>19.0375384625093</v>
+        <v>19.456902127582101</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B16">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="C16">
-        <v>49.4768830840842</v>
+        <v>54.035961601523603</v>
       </c>
       <c r="D16">
-        <v>20.0310572065559</v>
+        <v>19.0375384625093</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B17">
-        <v>300</v>
+        <v>120</v>
       </c>
       <c r="C17">
-        <v>53.777324326216203</v>
+        <v>49.4768830840842</v>
       </c>
       <c r="D17">
-        <v>20.4784014616428</v>
+        <v>20.0310572065559</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B18">
-        <v>100</v>
+        <v>300</v>
       </c>
       <c r="C18">
-        <v>52.412865110744498</v>
+        <v>53.777324326216203</v>
       </c>
       <c r="D18">
-        <v>16.9037246467723</v>
+        <v>20.4784014616428</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B19">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="C19">
-        <v>51.416416194443997</v>
+        <v>52.412865110744498</v>
       </c>
       <c r="D19">
-        <v>21.971062518997901</v>
+        <v>16.9037246467723</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B20">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="C20">
-        <v>51.401767215290697</v>
+        <v>51.416416194443997</v>
       </c>
       <c r="D20">
-        <v>21.156719321709801</v>
+        <v>21.971062518997901</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B21">
-        <v>60</v>
+        <v>100</v>
       </c>
       <c r="C21">
-        <v>50.0420242754223</v>
+        <v>51.401767215290697</v>
       </c>
       <c r="D21">
-        <v>22.000126734332</v>
+        <v>21.156719321709801</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B22">
-        <v>200</v>
+        <v>60</v>
       </c>
       <c r="C22">
-        <v>50.685598143633399</v>
+        <v>50.0420242754223</v>
       </c>
       <c r="D22">
-        <v>21.7535057976866</v>
+        <v>22.000126734332</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B23">
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="C23">
-        <v>53.430698528979597</v>
+        <v>50.685598143633399</v>
       </c>
       <c r="D23">
-        <v>14.546344895681001</v>
+        <v>21.7535057976866</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B24">
-        <v>60</v>
+        <v>150</v>
       </c>
       <c r="C24">
-        <v>50.311141303768103</v>
+        <v>53.430698528979597</v>
       </c>
       <c r="D24">
-        <v>21.0784565396639</v>
+        <v>14.546344895681001</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B25">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="C25">
-        <v>50.826850193108299</v>
+        <v>50.311141303768103</v>
       </c>
       <c r="D25">
-        <v>15.5202922147539</v>
+        <v>21.0784565396639</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B26">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="C26">
-        <v>50.014336879337101</v>
+        <v>50.826850193108299</v>
       </c>
       <c r="D26">
-        <v>20.9851455467909</v>
+        <v>15.5202922147539</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B27">
-        <v>200</v>
+        <v>70</v>
       </c>
       <c r="C27">
-        <v>52.253036318969997</v>
+        <v>50.014336879337101</v>
       </c>
       <c r="D27">
-        <v>21.0268573158327</v>
+        <v>20.9851455467909</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B28">
-        <v>90</v>
+        <v>200</v>
       </c>
       <c r="C28">
-        <v>49.986673711622501</v>
+        <v>52.253036318969997</v>
       </c>
       <c r="D28">
-        <v>20.065249867968699</v>
+        <v>21.0268573158327</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B29">
-        <v>40</v>
+        <v>90</v>
       </c>
       <c r="C29">
-        <v>51.114127107702103</v>
+        <v>49.986673711622501</v>
       </c>
       <c r="D29">
-        <v>17.024821717546601</v>
+        <v>20.065249867968699</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B30">
-        <v>200</v>
+        <v>40</v>
       </c>
       <c r="C30">
-        <v>49.296488760661397</v>
+        <v>51.114127107702103</v>
       </c>
       <c r="D30">
-        <v>19.9484695138574</v>
+        <v>17.024821717546601</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
+        <v>32</v>
+      </c>
+      <c r="B31">
+        <v>200</v>
+      </c>
+      <c r="C31">
+        <v>49.296488760661397</v>
+      </c>
+      <c r="D31">
+        <v>19.9484695138574</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
         <v>33</v>
       </c>
-      <c r="B31">
+      <c r="B32">
         <v>300</v>
       </c>
-      <c r="C31">
+      <c r="C32">
         <v>50.722355342783899</v>
       </c>
-      <c r="D31">
+      <c r="D32">
         <v>23.2524605159008</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Depot added as initial and final localisation
</commit_message>
<xml_diff>
--- a/Locations.xlsx
+++ b/Locations.xlsx
@@ -8,17 +8,28 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e46eb1fa8f051fd0/Dokumenty/1_STUDIA/1_UEK/semestr3/Metody_metaheurystyczne/projekt/CVRP_python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="169" documentId="11_F25DC773A252ABDACC104851391E68845BDE58F6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7BDC91D2-381C-4020-80B0-8FE81F711A5F}"/>
+  <xr:revisionPtr revIDLastSave="171" documentId="11_F25DC773A252ABDACC104851391E68845BDE58F6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C939FB78-AAE9-4EE0-B3C8-BE109D83CFB1}"/>
   <bookViews>
-    <workbookView xWindow="25035" yWindow="4995" windowWidth="17685" windowHeight="12660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="24030" yWindow="5400" windowWidth="17685" windowHeight="14685" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -454,18 +465,18 @@
   <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.21875" customWidth="1"/>
-    <col min="4" max="4" width="14.21875" customWidth="1"/>
+    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -479,7 +490,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>34</v>
       </c>
@@ -493,7 +504,7 @@
         <v>19.937306291842098</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -507,7 +518,7 @@
         <v>23.1440492704264</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -521,7 +532,7 @@
         <v>19.043440866477699</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -535,7 +546,7 @@
         <v>19.400068642432299</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -549,7 +560,7 @@
         <v>18.6035054972849</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -563,7 +574,7 @@
         <v>18.5245412653586</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -577,7 +588,7 @@
         <v>18.673647759229901</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -591,7 +602,7 @@
         <v>20.961498232116998</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -605,7 +616,7 @@
         <v>19.018350500255998</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -619,7 +630,7 @@
         <v>20.627657351131202</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -633,7 +644,7 @@
         <v>21.7668695000851</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -647,7 +658,7 @@
         <v>20.951569207975901</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -661,7 +672,7 @@
         <v>22.570635490611799</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -675,7 +686,7 @@
         <v>19.456902127582101</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -689,7 +700,7 @@
         <v>19.0375384625093</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -703,7 +714,7 @@
         <v>20.0310572065559</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -717,7 +728,7 @@
         <v>20.4784014616428</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -731,7 +742,7 @@
         <v>16.9037246467723</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -745,7 +756,7 @@
         <v>21.971062518997901</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>22</v>
       </c>
@@ -759,7 +770,7 @@
         <v>21.156719321709801</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>23</v>
       </c>
@@ -773,7 +784,7 @@
         <v>22.000126734332</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>24</v>
       </c>
@@ -787,7 +798,7 @@
         <v>21.7535057976866</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>25</v>
       </c>
@@ -801,7 +812,7 @@
         <v>14.546344895681001</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>26</v>
       </c>
@@ -815,7 +826,7 @@
         <v>21.0784565396639</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>27</v>
       </c>
@@ -829,7 +840,7 @@
         <v>15.5202922147539</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>28</v>
       </c>
@@ -843,7 +854,7 @@
         <v>20.9851455467909</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>29</v>
       </c>
@@ -857,7 +868,7 @@
         <v>21.0268573158327</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>30</v>
       </c>
@@ -871,7 +882,7 @@
         <v>20.065249867968699</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>31</v>
       </c>
@@ -885,7 +896,7 @@
         <v>17.024821717546601</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>32</v>
       </c>
@@ -899,7 +910,7 @@
         <v>19.9484695138574</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>33</v>
       </c>

</xml_diff>